<commit_message>
update JSON and add vis
</commit_message>
<xml_diff>
--- a/04 extraction consolidation results.xlsx
+++ b/04 extraction consolidation results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac130903\Desktop\MDE4DT\2\1\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EB066-250B-483B-A11D-0DE8204ED070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEE6D9F-8CD2-4FAA-916B-D26B5385EBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction consolidation result" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="392">
   <si>
     <t>Title</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>AutomationML</t>
-  </si>
-  <si>
-    <t>structure</t>
   </si>
   <si>
     <t>AutomationML models</t>
@@ -974,9 +971,6 @@
   </si>
   <si>
     <t>cyber-physical spaces (3D topology) model</t>
-  </si>
-  <si>
-    <t>Bi-Directional Model Transformation</t>
   </si>
   <si>
     <t>DT is specific</t>
@@ -1460,17 +1454,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Ausgabe" xfId="4" builtinId="21"/>
-    <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Notiz" xfId="5" builtinId="10"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="29">
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1554,6 +1545,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1609,41 +1603,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}" name="Tabelle1" displayName="Tabelle1" ref="A1:Y79" totalsRowShown="0" headerRowDxfId="28" dataDxfId="0" headerRowBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}" name="Tabelle1" displayName="Tabelle1" ref="A1:Y79" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" totalsRowBorderDxfId="25">
   <autoFilter ref="A1:Y79" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}"/>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{E9EA00CB-767A-4E0F-9046-D9C305AB9BE1}" name="Title" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4944576F-D53E-412A-A718-8D15CEAC1F87}" name="DT Definition" dataDxfId="24"/>
-    <tableColumn id="20" xr3:uid="{CBABB8A1-00DB-4C7A-AC1E-41C4010C63ED}" name="virtual space" dataDxfId="23"/>
-    <tableColumn id="22" xr3:uid="{CBD659E4-5140-4C8F-9EB7-6044F524E690}" name="Kritzinger" dataDxfId="22"/>
-    <tableColumn id="23" xr3:uid="{40736154-6068-44CA-9B63-88344A4B54C4}" name="DT is specific" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{C9CCBD3A-27D3-450B-9595-44CB8E2811DA}" name="modeling language" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{532C571A-A3FD-4370-AAA4-C4F894A2F074}" name="note on modeling language" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{EB6C62BB-070B-4919-9AC2-DCEB8E7627FF}" name="model type" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{B0D219EE-0CED-43F8-94EA-21B9C6F43EA9}" name="model processing technique" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{F5C81335-1FDC-4C5A-A1A2-6A37BD409F8F}" name="model usage technique" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{50DB7CC0-00A8-49BF-BE2F-2FBEFD4DAD97}" name="source" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{67098055-7248-42BA-BA89-183AEB280879}" name="target" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1899C93D-B2A5-4F9B-A715-253BA332D22F}" name="purpose of MDE application" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{1AA673CF-3A3D-4A64-B616-95F7D0973171}" name="purpose of DT" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{DA1C9F80-FD4C-4F63-B688-544381E0FBE8}" name="DTPurposeCategory" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{6AEE8298-3C9A-4B38-8133-409F65E1CC23}" name="use case domain" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{9499E08A-7527-4E4A-B957-C9B652220340}" name="system lifecycle phase" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{D4F96103-B987-421B-BDA9-07A167BCE10D}" name="twinning target" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{AAD31C43-B8FA-403C-8972-6F365065F29E}" name="twin lifecycle phase" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{D1E76F89-678F-498B-97FD-493EF01FF81C}" name="purpose /expected benefit of using models" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{11854641-31A8-4B9D-B081-A9EF0517B63F}" name="ModelPurposeCategory" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{27981E42-41B7-4E59-812C-1FFEB850EB4E}" name="open challenges" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{B6BBF896-38D1-4F10-98BC-2570B7841C08}" name="Technological Readiness Level" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{7E4CD30B-5CBB-4532-9641-16A4E11AEFCD}" name="notes" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{EE727955-0840-49EF-BB36-A6E7966D74DD}" name="Use Case" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E9EA00CB-767A-4E0F-9046-D9C305AB9BE1}" name="Title" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4944576F-D53E-412A-A718-8D15CEAC1F87}" name="DT Definition" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{CBABB8A1-00DB-4C7A-AC1E-41C4010C63ED}" name="virtual space" dataDxfId="22"/>
+    <tableColumn id="22" xr3:uid="{CBD659E4-5140-4C8F-9EB7-6044F524E690}" name="Kritzinger" dataDxfId="21"/>
+    <tableColumn id="23" xr3:uid="{40736154-6068-44CA-9B63-88344A4B54C4}" name="DT is specific" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{C9CCBD3A-27D3-450B-9595-44CB8E2811DA}" name="modeling language" dataDxfId="19"/>
+    <tableColumn id="21" xr3:uid="{532C571A-A3FD-4370-AAA4-C4F894A2F074}" name="note on modeling language" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{EB6C62BB-070B-4919-9AC2-DCEB8E7627FF}" name="model type" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{B0D219EE-0CED-43F8-94EA-21B9C6F43EA9}" name="model processing technique" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{F5C81335-1FDC-4C5A-A1A2-6A37BD409F8F}" name="model usage technique" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{50DB7CC0-00A8-49BF-BE2F-2FBEFD4DAD97}" name="source" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{67098055-7248-42BA-BA89-183AEB280879}" name="target" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{1899C93D-B2A5-4F9B-A715-253BA332D22F}" name="purpose of MDE application" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{1AA673CF-3A3D-4A64-B616-95F7D0973171}" name="purpose of DT" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{DA1C9F80-FD4C-4F63-B688-544381E0FBE8}" name="DTPurposeCategory" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{6AEE8298-3C9A-4B38-8133-409F65E1CC23}" name="use case domain" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{9499E08A-7527-4E4A-B957-C9B652220340}" name="system lifecycle phase" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{D4F96103-B987-421B-BDA9-07A167BCE10D}" name="twinning target" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{AAD31C43-B8FA-403C-8972-6F365065F29E}" name="twin lifecycle phase" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{D1E76F89-678F-498B-97FD-493EF01FF81C}" name="purpose /expected benefit of using models" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{11854641-31A8-4B9D-B081-A9EF0517B63F}" name="ModelPurposeCategory" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{27981E42-41B7-4E59-812C-1FFEB850EB4E}" name="open challenges" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{B6BBF896-38D1-4F10-98BC-2570B7841C08}" name="Technological Readiness Level" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{7E4CD30B-5CBB-4532-9641-16A4E11AEFCD}" name="notes" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{EE727955-0840-49EF-BB36-A6E7966D74DD}" name="Use Case" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1941,36 +1935,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC3CDE2-2548-49E4-A153-B9B62C0D483B}">
   <dimension ref="A1:Y79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X69" sqref="X69"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.83984375" customWidth="1"/>
-    <col min="2" max="2" width="16.15625" customWidth="1"/>
-    <col min="3" max="3" width="15.41796875" customWidth="1"/>
-    <col min="4" max="4" width="15.15625" customWidth="1"/>
-    <col min="5" max="5" width="16.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="25.41796875" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="17.26171875" customWidth="1"/>
-    <col min="12" max="12" width="22.41796875" customWidth="1"/>
-    <col min="13" max="13" width="23.578125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
-    <col min="16" max="16" width="41.68359375" customWidth="1"/>
-    <col min="17" max="17" width="20.578125" customWidth="1"/>
-    <col min="18" max="18" width="30.578125" customWidth="1"/>
-    <col min="19" max="19" width="38.41796875" customWidth="1"/>
-    <col min="20" max="22" width="23.15625" customWidth="1"/>
+    <col min="16" max="16" width="41.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
+    <col min="18" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="38.42578125" customWidth="1"/>
+    <col min="20" max="22" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1978,19 +1972,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>3</v>
@@ -2014,7 +2008,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>10</v>
@@ -2032,7 +2026,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>15</v>
@@ -2047,7 +2041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
@@ -2055,27 +2049,27 @@
         <v>20</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>23</v>
@@ -2087,7 +2081,7 @@
         <v>25</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>26</v>
@@ -2105,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V2" s="12"/>
       <c r="W2" s="5" t="s">
@@ -2116,7 +2110,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -2125,10 +2119,10 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="5" t="s">
@@ -2159,50 +2153,50 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>27</v>
@@ -2214,10 +2208,10 @@
         <v>29</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="5" t="s">
@@ -2225,10 +2219,10 @@
       </c>
       <c r="X4" s="12"/>
       <c r="Y4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>35</v>
       </c>
@@ -2239,30 +2233,30 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="S5" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
@@ -2271,28 +2265,28 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>22</v>
@@ -2302,22 +2296,22 @@
         <v>33</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>28</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
@@ -2327,46 +2321,46 @@
       </c>
       <c r="X6" s="12"/>
       <c r="Y6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -2375,9 +2369,9 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2388,30 +2382,30 @@
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>64</v>
-      </c>
       <c r="Q8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>28</v>
@@ -2420,10 +2414,10 @@
         <v>29</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="V8" s="12"/>
       <c r="W8" s="5" t="s">
@@ -2431,42 +2425,42 @@
       </c>
       <c r="X8" s="12"/>
       <c r="Y8" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="12" t="s">
@@ -2479,30 +2473,30 @@
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F10" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>268</v>
-      </c>
       <c r="H10" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -2522,59 +2516,59 @@
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="M11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="O11" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R11" s="12" t="s">
         <v>28</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
@@ -2585,9 +2579,9 @@
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -2596,28 +2590,28 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="L12" s="12" t="s">
         <v>297</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>298</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
@@ -2626,72 +2620,72 @@
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="M13" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S13" s="12" t="s">
         <v>29</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="V13" s="12"/>
       <c r="W13" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -2700,17 +2694,17 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
@@ -2730,52 +2724,52 @@
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="L15" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="M15" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="N15" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="N15" s="12" t="s">
+      <c r="O15" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="P15" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="O15" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>27</v>
@@ -2787,55 +2781,55 @@
         <v>29</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="V15" s="12"/>
       <c r="W15" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="Y15" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="12" t="s">
@@ -2848,53 +2842,53 @@
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R17" s="12" t="s">
         <v>28</v>
@@ -2911,9 +2905,9 @@
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -2921,27 +2915,27 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="12" t="s">
@@ -2954,63 +2948,63 @@
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="O19" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="R19" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="S19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="T19" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="U19" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="V19" s="12"/>
       <c r="W19" s="5" t="s">
@@ -3018,88 +3012,88 @@
       </c>
       <c r="X19" s="12"/>
       <c r="Y19" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="C20" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="M20" s="12"/>
       <c r="N20" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S20" s="12" t="s">
         <v>29</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="V20" s="12"/>
       <c r="W20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="X20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="Y20" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -3121,16 +3115,16 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -3152,112 +3146,112 @@
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="M23" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="M23" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="O23" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R23" s="12" t="s">
         <v>28</v>
       </c>
       <c r="S23" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="V23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="U23" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="V23" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="W23" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X23" s="12"/>
       <c r="Y23" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
@@ -3266,41 +3260,41 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25" s="12" t="s">
         <v>128</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>129</v>
       </c>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
@@ -3309,41 +3303,41 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="L26" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T26" s="12"/>
       <c r="U26" s="12"/>
@@ -3352,41 +3346,41 @@
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
@@ -3395,41 +3389,41 @@
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L28" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
@@ -3438,41 +3432,41 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L29" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T29" s="12"/>
       <c r="U29" s="12"/>
@@ -3481,41 +3475,41 @@
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="L30" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q30" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R30" s="12" t="s">
         <v>28</v>
@@ -3524,10 +3518,10 @@
         <v>29</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="V30" s="12"/>
       <c r="W30" s="5" t="s">
@@ -3535,40 +3529,40 @@
       </c>
       <c r="X30" s="12"/>
       <c r="Y30" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="12" t="s">
@@ -3581,9 +3575,9 @@
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -3592,24 +3586,24 @@
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="12" t="s">
@@ -3622,51 +3616,51 @@
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="M33" s="12"/>
       <c r="N33" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O33" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q33" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="12" t="s">
@@ -3675,64 +3669,64 @@
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
       <c r="V33" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W33" s="5" t="s">
         <v>31</v>
       </c>
       <c r="X33" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F34" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>270</v>
-      </c>
       <c r="H34" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S34" s="12" t="s">
         <v>29</v>
@@ -3740,7 +3734,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
       <c r="V34" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W34" s="5" t="s">
         <v>31</v>
@@ -3748,16 +3742,16 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -3779,53 +3773,53 @@
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>94</v>
-      </c>
       <c r="I36" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L36" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="M36" s="12"/>
       <c r="N36" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O36" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P36" s="12" t="s">
         <v>26</v>
       </c>
       <c r="Q36" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R36" s="12" t="s">
         <v>28</v>
@@ -3842,9 +3836,9 @@
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -3853,24 +3847,24 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="12" t="s">
@@ -3883,43 +3877,43 @@
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L38" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>162</v>
       </c>
       <c r="M38" s="12"/>
       <c r="N38" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P38" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q38" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R38" s="12" t="s">
         <v>28</v>
@@ -3935,40 +3929,40 @@
       </c>
       <c r="X38" s="12"/>
       <c r="Y38" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="L39" s="12" t="s">
         <v>165</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R39" s="12"/>
       <c r="S39" s="12" t="s">
@@ -3981,19 +3975,19 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="G40" s="12" t="s">
         <v>273</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>274</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -4014,21 +4008,21 @@
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="C41" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>21</v>
@@ -4036,58 +4030,58 @@
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L41" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M41" s="12"/>
       <c r="N41" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q41" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R41" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R41" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="S41" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T41" s="12"/>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
       <c r="W41" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X41" s="12"/>
       <c r="Y41" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
@@ -4108,53 +4102,53 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="C43" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P43" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q43" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R43" s="12" t="s">
         <v>28</v>
@@ -4163,10 +4157,10 @@
         <v>29</v>
       </c>
       <c r="T43" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U43" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V43" s="12"/>
       <c r="W43" s="5" t="s">
@@ -4175,37 +4169,37 @@
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="12" t="s">
@@ -4218,44 +4212,44 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>178</v>
-      </c>
       <c r="C45" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L45" s="12" t="s">
         <v>180</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>181</v>
       </c>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
       <c r="P45" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q45" s="12" t="s">
         <v>27</v>
@@ -4265,13 +4259,13 @@
         <v>29</v>
       </c>
       <c r="T45" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="U45" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="V45" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="U45" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="V45" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="W45" s="5" t="s">
         <v>31</v>
@@ -4282,37 +4276,37 @@
         <v>automatic fire extinguishing system</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R46" s="12" t="s">
         <v>28</v>
@@ -4327,37 +4321,37 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="12" t="s">
@@ -4370,37 +4364,37 @@
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M48" s="12"/>
       <c r="N48" s="12"/>
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R48" s="12"/>
       <c r="S48" s="12" t="s">
@@ -4413,37 +4407,37 @@
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="L49" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="M49" s="12"/>
       <c r="N49" s="12"/>
       <c r="O49" s="12"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R49" s="12"/>
       <c r="S49" s="12" t="s">
@@ -4456,54 +4450,54 @@
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>194</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>195</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>312</v>
+        <v>22</v>
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="L50" s="12" t="s">
         <v>310</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>311</v>
       </c>
       <c r="M50" s="12"/>
       <c r="N50" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="P50" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="O50" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="P50" s="12" t="s">
+      <c r="Q50" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="Q50" s="12" t="s">
-        <v>198</v>
-      </c>
       <c r="R50" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S50" s="12" t="s">
         <v>29</v>
@@ -4511,52 +4505,52 @@
       <c r="T50" s="12"/>
       <c r="U50" s="12"/>
       <c r="V50" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W50" s="5" t="s">
         <v>31</v>
       </c>
       <c r="X50" s="12"/>
       <c r="Y50" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="H51" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="L51" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="M51" s="12"/>
       <c r="N51" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O51" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P51" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q51" s="12" t="s">
         <v>27</v>
@@ -4574,13 +4568,13 @@
         <v>31</v>
       </c>
       <c r="X51" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y51" s="12"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -4589,17 +4583,17 @@
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M52" s="12"/>
       <c r="N52" s="12"/>
@@ -4619,38 +4613,38 @@
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>207</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>208</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="L53" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>209</v>
       </c>
       <c r="M53" s="12"/>
       <c r="N53" s="12"/>
@@ -4659,7 +4653,7 @@
         <v>26</v>
       </c>
       <c r="Q53" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R53" s="12" t="s">
         <v>28</v>
@@ -4675,43 +4669,43 @@
       </c>
       <c r="X53" s="12"/>
       <c r="Y53" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I54" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="L54" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="L54" s="12" t="s">
-        <v>214</v>
       </c>
       <c r="M54" s="12"/>
       <c r="N54" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O54" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P54" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q54" s="12" t="s">
         <v>27</v>
@@ -4728,33 +4722,33 @@
       </c>
       <c r="X54" s="12"/>
       <c r="Y54" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I55" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L55" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M55" s="12"/>
       <c r="N55" s="12"/>
@@ -4774,30 +4768,30 @@
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L56" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>218</v>
       </c>
       <c r="M56" s="12"/>
       <c r="N56" s="12"/>
@@ -4817,32 +4811,32 @@
       <c r="X56" s="12"/>
       <c r="Y56" s="12"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="G57" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="G57" s="12" t="s">
-        <v>279</v>
-      </c>
       <c r="H57" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="L57" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="M57" s="12"/>
       <c r="N57" s="12"/>
@@ -4862,56 +4856,56 @@
       <c r="X57" s="12"/>
       <c r="Y57" s="12"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L58" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="N58" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="M58" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="N58" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="O58" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q58" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R58" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S58" s="12" t="s">
         <v>29</v>
@@ -4924,33 +4918,33 @@
       </c>
       <c r="X58" s="12"/>
       <c r="Y58" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J59" s="12"/>
       <c r="K59" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M59" s="12"/>
       <c r="N59" s="12"/>
@@ -4970,16 +4964,16 @@
       <c r="X59" s="12"/>
       <c r="Y59" s="12"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -5001,47 +4995,47 @@
       <c r="X60" s="12"/>
       <c r="Y60" s="12"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L61" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M61" s="12"/>
       <c r="N61" s="12"/>
       <c r="O61" s="12"/>
       <c r="P61" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q61" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R61" s="12" t="s">
         <v>28</v>
@@ -5050,10 +5044,10 @@
         <v>29</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U61" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V61" s="12"/>
       <c r="W61" s="5" t="s">
@@ -5062,37 +5056,37 @@
       <c r="X61" s="12"/>
       <c r="Y61" s="12"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J62" s="12"/>
       <c r="K62" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L62" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M62" s="12"/>
       <c r="N62" s="12"/>
       <c r="O62" s="12"/>
       <c r="P62" s="12"/>
       <c r="Q62" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R62" s="12"/>
       <c r="S62" s="12" t="s">
@@ -5105,37 +5099,37 @@
       <c r="X62" s="12"/>
       <c r="Y62" s="12"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L63" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M63" s="12"/>
       <c r="N63" s="12"/>
       <c r="O63" s="12"/>
       <c r="P63" s="12"/>
       <c r="Q63" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R63" s="12"/>
       <c r="S63" s="12" t="s">
@@ -5148,59 +5142,59 @@
       <c r="X63" s="12"/>
       <c r="Y63" s="12"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="C64" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F64" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="G64" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G64" s="12" t="s">
-        <v>282</v>
-      </c>
       <c r="H64" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="L64" s="12" t="s">
         <v>235</v>
-      </c>
-      <c r="L64" s="12" t="s">
-        <v>236</v>
       </c>
       <c r="M64" s="12"/>
       <c r="N64" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O64" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P64" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q64" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R64" s="12" t="s">
         <v>28</v>
       </c>
       <c r="S64" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="T64" s="12"/>
       <c r="U64" s="12"/>
@@ -5209,57 +5203,57 @@
         <v>31</v>
       </c>
       <c r="X64" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y64" s="12"/>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="Y64" s="12"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="10" t="s">
+      <c r="B65" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F65" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>241</v>
-      </c>
       <c r="G65" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H65" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="L65" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="L65" s="12" t="s">
-        <v>242</v>
       </c>
       <c r="M65" s="12"/>
       <c r="N65" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O65" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P65" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q65" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R65" s="12" t="s">
         <v>28</v>
@@ -5276,59 +5270,59 @@
       <c r="X65" s="12"/>
       <c r="Y65" s="12"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="C66" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="G66" s="12"/>
       <c r="H66" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="L66" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="L66" s="12" t="s">
+      <c r="M66" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="N66" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="M66" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="N66" s="5" t="s">
-        <v>249</v>
-      </c>
       <c r="O66" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P66" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q66" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R66" s="12" t="s">
         <v>28</v>
       </c>
       <c r="S66" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T66" s="12"/>
       <c r="U66" s="12"/>
@@ -5338,12 +5332,12 @@
       </c>
       <c r="X66" s="12"/>
       <c r="Y66" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -5352,28 +5346,28 @@
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L67" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M67" s="12"/>
       <c r="N67" s="12"/>
       <c r="O67" s="12"/>
       <c r="P67" s="12"/>
       <c r="Q67" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R67" s="12"/>
       <c r="S67" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T67" s="12"/>
       <c r="U67" s="12"/>
@@ -5382,53 +5376,53 @@
       <c r="X67" s="12"/>
       <c r="Y67" s="12"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="C68" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F68" s="12" t="s">
         <v>253</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>254</v>
       </c>
       <c r="G68" s="12"/>
       <c r="H68" s="12" t="s">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L68" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M68" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="N68" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="N68" s="5" t="s">
-        <v>257</v>
-      </c>
       <c r="O68" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P68" s="12" t="s">
         <v>26</v>
       </c>
       <c r="Q68" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R68" s="12"/>
       <c r="S68" s="12" t="s">
@@ -5442,93 +5436,93 @@
       </c>
       <c r="X68" s="12"/>
       <c r="Y68" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G69" s="12"/>
       <c r="H69" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I69" t="s">
         <v>22</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L69" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M69" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="N69" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="O69" s="12"/>
       <c r="P69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q69" t="s">
         <v>27</v>
       </c>
       <c r="R69" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S69" t="s">
         <v>29</v>
       </c>
       <c r="T69" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="U69" s="12"/>
       <c r="W69" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="X69" s="12"/>
       <c r="Y69" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
       <c r="F70" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G70" s="12"/>
       <c r="H70" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J70" s="12"/>
       <c r="O70" s="12"/>
       <c r="U70" s="12"/>
       <c r="X70" s="12"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
@@ -5536,187 +5530,187 @@
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="I71" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L71" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="M71" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="O71" s="12"/>
       <c r="P71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q71" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="R71" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S71" t="s">
         <v>29</v>
       </c>
       <c r="T71" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="U71" s="12"/>
       <c r="W71" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="X71" s="12"/>
       <c r="Y71" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G72" s="12"/>
       <c r="H72" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L72" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="M72" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N72" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="O72" s="12"/>
       <c r="P72" t="s">
         <v>26</v>
       </c>
       <c r="Q72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R72" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T72" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="U72" s="12"/>
       <c r="V72" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="W72" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="X72" s="12"/>
       <c r="Y72" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G73" s="12"/>
       <c r="H73" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I73" t="s">
         <v>22</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L73" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="M73" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N73" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O73" s="12"/>
       <c r="P73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q73" t="s">
         <v>27</v>
       </c>
       <c r="R73" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S73" t="s">
         <v>29</v>
       </c>
       <c r="U73" s="12"/>
       <c r="W73" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="X73" s="12"/>
       <c r="Y73" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G74" s="12"/>
       <c r="H74" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I74" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L74" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O74" s="12"/>
       <c r="Q74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S74" t="s">
         <v>29</v>
@@ -5724,18 +5718,18 @@
       <c r="U74" s="12"/>
       <c r="X74" s="12"/>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G75" s="12"/>
       <c r="I75" t="s">
@@ -5743,67 +5737,67 @@
       </c>
       <c r="J75" s="12"/>
       <c r="K75" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M75" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="N75" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="O75" s="12"/>
       <c r="P75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q75" t="s">
         <v>27</v>
       </c>
       <c r="R75" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S75" t="s">
         <v>29</v>
       </c>
       <c r="T75" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="U75" s="12"/>
       <c r="W75" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="X75" s="12"/>
       <c r="Y75" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
       <c r="F76" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G76" s="12"/>
       <c r="I76" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J76" s="12"/>
       <c r="K76" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L76" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="O76" s="12"/>
       <c r="Q76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S76" t="s">
         <v>29</v>
@@ -5811,9 +5805,9 @@
       <c r="U76" s="12"/>
       <c r="X76" s="12"/>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
@@ -5822,18 +5816,18 @@
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
       <c r="I77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L77" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="O77" s="12"/>
       <c r="Q77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S77" t="s">
         <v>29</v>
@@ -5841,9 +5835,9 @@
       <c r="U77" s="12"/>
       <c r="X77" s="12"/>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -5852,18 +5846,18 @@
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
       <c r="I78" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L78" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="O78" s="12"/>
       <c r="Q78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S78" t="s">
         <v>29</v>
@@ -5871,7 +5865,7 @@
       <c r="U78" s="12"/>
       <c r="X78" s="12"/>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>

</xml_diff>

<commit_message>
update reference IDs after adding new papers
</commit_message>
<xml_diff>
--- a/04 extraction consolidation results.xlsx
+++ b/04 extraction consolidation results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA252110-CF54-400A-A449-B4EE11768C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721834E2-564A-472F-9900-A25E0C5F86B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction consolidation result" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="450">
   <si>
     <t>Title</t>
   </si>
@@ -1300,9 +1300,6 @@
     <t>S45</t>
   </si>
   <si>
-    <t>S61</t>
-  </si>
-  <si>
     <t>S6</t>
   </si>
   <si>
@@ -1315,9 +1312,6 @@
     <t>S13</t>
   </si>
   <si>
-    <t>S27</t>
-  </si>
-  <si>
     <t>S40</t>
   </si>
   <si>
@@ -1382,6 +1376,15 @@
   </si>
   <si>
     <t>maintenance platform</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>S65</t>
+  </si>
+  <si>
+    <t>S66</t>
   </si>
 </sst>
 </file>
@@ -2344,21 +2347,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O137" sqref="O137"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="114.3125" customWidth="1"/>
-    <col min="4" max="4" width="42.1015625" customWidth="1"/>
+    <col min="3" max="3" width="114.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="23.1015625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.3125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
         <v>356</v>
       </c>
@@ -2383,7 +2386,7 @@
       </c>
       <c r="T1" s="12"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>205</v>
       </c>
@@ -2445,12 +2448,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>375</v>
+        <v>449</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>209</v>
@@ -2498,12 +2501,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>375</v>
+        <v>449</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>209</v>
@@ -2536,12 +2539,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2589,12 +2592,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2627,12 +2630,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>20</v>
@@ -2680,12 +2683,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>20</v>
@@ -2718,12 +2721,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>378</v>
+        <v>407</v>
       </c>
       <c r="C9" t="s">
         <v>220</v>
@@ -2765,7 +2768,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -2900,12 +2903,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C13" t="s">
         <v>224</v>
@@ -2959,12 +2962,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C14" t="s">
         <v>224</v>
@@ -3003,12 +3006,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>7</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>381</v>
+        <v>416</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>35</v>
@@ -3059,12 +3062,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>381</v>
+        <v>416</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>35</v>
@@ -3100,7 +3103,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>9</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -3206,12 +3209,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C19" t="s">
         <v>42</v>
@@ -3247,12 +3250,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>11</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>165</v>
@@ -3306,7 +3309,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3400,12 +3403,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>13</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>233</v>
@@ -3453,7 +3456,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
@@ -3506,7 +3509,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>15</v>
       </c>
@@ -3559,12 +3562,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
@@ -3609,12 +3612,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="C27" t="s">
         <v>96</v>
@@ -3647,7 +3650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>17</v>
       </c>
@@ -3697,12 +3700,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="C29" t="s">
         <v>63</v>
@@ -3753,7 +3756,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>19</v>
       </c>
@@ -3806,7 +3809,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
@@ -3859,7 +3862,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
@@ -3935,7 +3938,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20</v>
       </c>
@@ -4011,7 +4014,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20</v>
       </c>
@@ -4049,7 +4052,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20</v>
       </c>
@@ -4087,7 +4090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>21</v>
       </c>
@@ -4143,12 +4146,12 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>22</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>85</v>
@@ -4199,12 +4202,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>22</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>85</v>
@@ -4237,12 +4240,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>22</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>85</v>
@@ -4275,7 +4278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>23</v>
       </c>
@@ -4319,7 +4322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>24</v>
       </c>
@@ -4372,12 +4375,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>25</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>55</v>
@@ -4422,12 +4425,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>25</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>55</v>
@@ -4460,7 +4463,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>26</v>
       </c>
@@ -4513,7 +4516,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>26</v>
       </c>
@@ -4557,12 +4560,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>27</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>400</v>
+        <v>448</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>103</v>
@@ -4613,7 +4616,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>28</v>
       </c>
@@ -4663,7 +4666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>28</v>
       </c>
@@ -4701,12 +4704,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>29</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>110</v>
@@ -4754,12 +4757,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>29</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>110</v>
@@ -4795,12 +4798,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>29</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>110</v>
@@ -4836,12 +4839,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>29</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>110</v>
@@ -4874,12 +4877,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>29</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>110</v>
@@ -4912,12 +4915,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>30</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>403</v>
+        <v>375</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>119</v>
@@ -4968,7 +4971,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>31</v>
       </c>
@@ -5012,7 +5015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>31</v>
       </c>
@@ -5050,7 +5053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>31</v>
       </c>
@@ -5088,12 +5091,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>32</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>125</v>
@@ -5132,12 +5135,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>32</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>125</v>
@@ -5170,7 +5173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>33</v>
       </c>
@@ -5223,12 +5226,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>34</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>407</v>
+        <v>422</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>169</v>
@@ -5279,12 +5282,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>35</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>133</v>
@@ -5332,12 +5335,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>35</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>133</v>
@@ -5370,12 +5373,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:20" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>35</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>133</v>
@@ -5408,12 +5411,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>35</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>133</v>
@@ -5449,12 +5452,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:20" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:20" s="7" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>36</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>409</v>
+        <v>380</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>174</v>
@@ -5502,12 +5505,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="69" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>37</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>178</v>
@@ -5555,12 +5558,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>37</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>178</v>
@@ -5596,12 +5599,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>38</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>256</v>
@@ -5640,12 +5643,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>38</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>256</v>
@@ -5678,12 +5681,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>38</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>256</v>
@@ -5719,12 +5722,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>39</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>260</v>
@@ -5772,12 +5775,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>40</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>141</v>
@@ -5828,12 +5831,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>40</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>141</v>
@@ -5869,7 +5872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>41</v>
       </c>
@@ -5919,7 +5922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>41</v>
       </c>
@@ -5957,7 +5960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>41</v>
       </c>
@@ -5995,7 +5998,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>42</v>
       </c>
@@ -6042,12 +6045,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>152</v>
@@ -6092,12 +6095,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>44</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>183</v>
@@ -6148,12 +6151,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>44</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>183</v>
@@ -6186,12 +6189,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>44</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>183</v>
@@ -6224,12 +6227,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>44</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>183</v>
@@ -6265,12 +6268,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="5" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:20" s="5" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>45</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>155</v>
@@ -6318,12 +6321,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>45</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>155</v>
@@ -6359,12 +6362,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>46</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>262</v>
@@ -6412,12 +6415,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>46</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>262</v>
@@ -6450,12 +6453,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>47</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>161</v>
@@ -6500,12 +6503,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>48</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>421</v>
+        <v>384</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>268</v>
@@ -6550,12 +6553,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>48</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>421</v>
+        <v>384</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>268</v>
@@ -6588,12 +6591,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>48</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>421</v>
+        <v>384</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>268</v>
@@ -6626,12 +6629,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>49</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>272</v>
@@ -6682,12 +6685,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>49</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>272</v>
@@ -6723,12 +6726,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>49</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>272</v>
@@ -6761,12 +6764,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>50</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>278</v>
@@ -6814,12 +6817,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="98" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>50</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>278</v>
@@ -6852,12 +6855,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>50</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>278</v>
@@ -6890,12 +6893,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>50</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>278</v>
@@ -6928,12 +6931,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>51</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>288</v>
@@ -6981,12 +6984,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="102" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>51</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>288</v>
@@ -7022,12 +7025,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>52</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>295</v>
@@ -7078,12 +7081,12 @@
         <v>298</v>
       </c>
     </row>
-    <row r="104" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>52</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>295</v>
@@ -7116,12 +7119,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>53</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>426</v>
+        <v>391</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>301</v>
@@ -7160,12 +7163,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="106" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>54</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>427</v>
+        <v>386</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>305</v>
@@ -7216,12 +7219,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="107" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>54</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>427</v>
+        <v>386</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>305</v>
@@ -7257,12 +7260,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>55</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>311</v>
@@ -7307,12 +7310,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>55</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>311</v>
@@ -7345,12 +7348,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>56</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>315</v>
@@ -7389,12 +7392,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>56</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>315</v>
@@ -7427,12 +7430,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>56</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>315</v>
@@ -7465,12 +7468,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="113" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>56</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>315</v>
@@ -7503,12 +7506,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>56</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>315</v>
@@ -7541,12 +7544,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>56</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>315</v>
@@ -7579,12 +7582,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>56</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>315</v>
@@ -7614,12 +7617,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>56</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>315</v>
@@ -7652,12 +7655,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>56</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>315</v>
@@ -7690,12 +7693,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="119" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>57</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>324</v>
@@ -7737,12 +7740,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>57</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>324</v>
@@ -7775,12 +7778,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>58</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>328</v>
@@ -7822,12 +7825,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>58</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>328</v>
@@ -7863,12 +7866,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>58</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>328</v>
@@ -7904,12 +7907,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>59</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>432</v>
+        <v>377</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>330</v>
@@ -7957,12 +7960,12 @@
         <v>333</v>
       </c>
     </row>
-    <row r="125" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>59</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>432</v>
+        <v>377</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>330</v>
@@ -7998,12 +8001,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>59</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>432</v>
+        <v>377</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>330</v>
@@ -8039,12 +8042,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>60</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>336</v>
@@ -8095,12 +8098,12 @@
         <v>339</v>
       </c>
     </row>
-    <row r="128" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>61</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>340</v>
@@ -8148,12 +8151,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="129" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>61</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>340</v>
@@ -8189,12 +8192,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="130" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>61</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>340</v>
@@ -8227,12 +8230,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>62</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>344</v>
@@ -8283,12 +8286,12 @@
         <v>347</v>
       </c>
     </row>
-    <row r="132" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
         <v>63</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>348</v>
@@ -8339,12 +8342,12 @@
         <v>351</v>
       </c>
     </row>
-    <row r="133" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>64</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>352</v>
@@ -8392,18 +8395,21 @@
         <v>355</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
         <v>65</v>
       </c>
+      <c r="B134" s="5" t="s">
+        <v>411</v>
+      </c>
       <c r="C134" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E134" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F134" t="s">
         <v>195</v>
@@ -8415,7 +8421,7 @@
         <v>198</v>
       </c>
       <c r="J134" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K134" t="s">
         <v>196</v>
@@ -8430,33 +8436,36 @@
         <v>304</v>
       </c>
       <c r="P134" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q134" s="7" t="s">
         <v>29</v>
       </c>
       <c r="R134" t="s">
+        <v>440</v>
+      </c>
+      <c r="S134" t="s">
+        <v>441</v>
+      </c>
+      <c r="T134" t="s">
         <v>442</v>
       </c>
-      <c r="S134" t="s">
-        <v>443</v>
-      </c>
-      <c r="T134" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
         <v>65</v>
       </c>
+      <c r="B135" s="5" t="s">
+        <v>411</v>
+      </c>
       <c r="C135" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E135" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F135" t="s">
         <v>195</v>
@@ -8468,7 +8477,7 @@
         <v>198</v>
       </c>
       <c r="J135" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K135" t="s">
         <v>197</v>
@@ -8478,28 +8487,30 @@
       </c>
       <c r="N135" s="7"/>
       <c r="P135" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q135" s="7" t="s">
         <v>29</v>
       </c>
       <c r="R135" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>66</v>
       </c>
-      <c r="B136" s="5"/>
+      <c r="B136" s="5" t="s">
+        <v>400</v>
+      </c>
       <c r="C136" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F136" s="5" t="s">
         <v>195</v>
@@ -8512,7 +8523,7 @@
         <v>198</v>
       </c>
       <c r="J136" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>197</v>
@@ -8526,7 +8537,7 @@
         <v>304</v>
       </c>
       <c r="P136" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q136" s="5" t="s">
         <v>15</v>
@@ -8536,7 +8547,7 @@
       </c>
       <c r="S136" s="5"/>
       <c r="T136" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -8545,8 +8556,8 @@
       <sortCondition ref="A2:A68"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:T133">
-    <sortCondition ref="A2:A133"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:T136">
+    <sortCondition ref="A2:A136"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="D1:O1"/>

</xml_diff>

<commit_message>
delete filters from excel files
</commit_message>
<xml_diff>
--- a/04 extraction consolidation results.xlsx
+++ b/04 extraction consolidation results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Repos\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721834E2-564A-472F-9900-A25E0C5F86B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0923C6-EBDC-4D71-AA6F-FAF2A2581F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction consolidation result" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="450">
   <si>
     <t>Title</t>
   </si>
@@ -1354,12 +1354,6 @@
     <t>simulation model</t>
   </si>
   <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>as-designed</t>
-  </si>
-  <si>
     <t>Human heath and social work activities</t>
   </si>
   <si>
@@ -1385,6 +1379,12 @@
   </si>
   <si>
     <t>S66</t>
+  </si>
+  <si>
+    <t>Soft Gripper System</t>
+  </si>
+  <si>
+    <t>Storage System</t>
   </si>
 </sst>
 </file>
@@ -2347,9 +2347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>209</v>
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>209</v>
@@ -4321,6 +4321,9 @@
       <c r="R42" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="S42" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="43" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -4565,7 +4568,7 @@
         <v>27</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>103</v>
@@ -5604,7 +5607,7 @@
         <v>38</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>256</v>
@@ -5648,7 +5651,7 @@
         <v>38</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>256</v>
@@ -5686,7 +5689,7 @@
         <v>38</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>256</v>
@@ -6044,6 +6047,12 @@
       <c r="R80" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="S80" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T80" s="7" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="81" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
@@ -7739,6 +7748,12 @@
       <c r="R119" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="S119" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T119" s="5" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="120" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
@@ -8421,7 +8436,7 @@
         <v>198</v>
       </c>
       <c r="J134" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K134" t="s">
         <v>196</v>
@@ -8436,19 +8451,19 @@
         <v>304</v>
       </c>
       <c r="P134" t="s">
-        <v>439</v>
+        <v>28</v>
       </c>
       <c r="Q134" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R134" t="s">
+      <c r="R134" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S134" t="s">
+        <v>439</v>
+      </c>
+      <c r="T134" t="s">
         <v>440</v>
-      </c>
-      <c r="S134" t="s">
-        <v>441</v>
-      </c>
-      <c r="T134" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
@@ -8477,7 +8492,7 @@
         <v>198</v>
       </c>
       <c r="J135" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K135" t="s">
         <v>197</v>
@@ -8487,13 +8502,10 @@
       </c>
       <c r="N135" s="7"/>
       <c r="P135" t="s">
-        <v>439</v>
+        <v>28</v>
       </c>
       <c r="Q135" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="R135" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
@@ -8523,7 +8535,7 @@
         <v>198</v>
       </c>
       <c r="J136" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>197</v>
@@ -8537,7 +8549,7 @@
         <v>304</v>
       </c>
       <c r="P136" s="5" t="s">
-        <v>439</v>
+        <v>28</v>
       </c>
       <c r="Q136" s="5" t="s">
         <v>15</v>
@@ -8547,7 +8559,7 @@
       </c>
       <c r="S136" s="5"/>
       <c r="T136" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>